<commit_message>
Major progress: preliminary mark-to-market setup, simulation runs, major data structuring, and cleanup. Big push today.
</commit_message>
<xml_diff>
--- a/data/bbva_calculator_values.xlsx
+++ b/data/bbva_calculator_values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauricio\Code\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauricio\Code\Autocalls\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53F1B0-2CF7-4C92-A74C-FBFACFD00ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AE9810-D86B-41AD-843F-1442562E5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="14610" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>This is the default configuration for our testing. We also assume that the internal Actinver team used this configuration when pricing their autocalls in the past</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Ticker/Index Name: 27/05/2025 14:10-14:28</t>
+  </si>
+  <si>
+    <t>Ticker/Index Name: 29/05/2025 14:15-14:30</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,6 +793,38 @@
         <v>3.1711499999999999</v>
       </c>
     </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>10.49249</v>
+      </c>
+      <c r="C12">
+        <v>16.088978999999998</v>
+      </c>
+      <c r="D12">
+        <v>12.423120000000001</v>
+      </c>
+      <c r="E12">
+        <v>6.8448929999999999</v>
+      </c>
+      <c r="F12">
+        <v>4.4332510000000003</v>
+      </c>
+      <c r="G12">
+        <v>4.535018</v>
+      </c>
+      <c r="H12">
+        <v>3.6621779999999999</v>
+      </c>
+      <c r="I12">
+        <v>4.4559819999999997</v>
+      </c>
+      <c r="J12">
+        <v>3.2815639999999999</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:N1"/>

</xml_diff>

<commit_message>
Spoke With Gus and Updated BBVA table
</commit_message>
<xml_diff>
--- a/data/bbva_calculator_values.xlsx
+++ b/data/bbva_calculator_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauricio\Code\Autocalls\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AE9810-D86B-41AD-843F-1442562E5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE98189-EA19-4072-A008-3F698D6ACD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="14610" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16200" windowHeight="10102" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>This is the default configuration for our testing. We also assume that the internal Actinver team used this configuration when pricing their autocalls in the past</t>
   </si>
@@ -104,13 +104,16 @@
   </si>
   <si>
     <t>Ticker/Index Name: 29/05/2025 14:15-14:30</t>
+  </si>
+  <si>
+    <t>Ticker/Index Name: 29/05/2025 15:30-16:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +123,12 @@
     </font>
     <font>
       <sz val="19"/>
+      <color rgb="FF7E7E7E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF7E7E7E"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -151,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,6 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,18 +500,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -519,7 +529,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -560,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -598,7 +608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -645,12 +655,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -682,12 +692,12 @@
         <v>3.34518</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -725,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="23.65" x14ac:dyDescent="0.6">
       <c r="B9" s="2">
         <v>10.370602</v>
       </c>
@@ -761,7 +771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="23.65" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -793,7 +803,7 @@
         <v>3.1711499999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -823,6 +833,38 @@
       </c>
       <c r="J12">
         <v>3.2815639999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10.533529</v>
+      </c>
+      <c r="C13">
+        <v>15.760683</v>
+      </c>
+      <c r="D13" s="5">
+        <v>12.350709</v>
+      </c>
+      <c r="E13">
+        <v>6.705165</v>
+      </c>
+      <c r="F13" s="5">
+        <v>4.3503759999999998</v>
+      </c>
+      <c r="G13" s="5">
+        <v>4.4639420000000003</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3.702788</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>